<commit_message>
changes to parameter table & input for multiple species simulations
</commit_message>
<xml_diff>
--- a/Parameter Table.xlsx
+++ b/Parameter Table.xlsx
@@ -1116,9 +1116,6 @@
     <t>Shape parameter 2 of beta distribution of wind strength</t>
   </si>
   <si>
-    <t>Number of days for 100% of the water body nutrients to mix</t>
-  </si>
-  <si>
     <t>Water body characteristic</t>
   </si>
   <si>
@@ -1195,6 +1192,9 @@
   </si>
   <si>
     <t>Submerged plant biomass</t>
+  </si>
+  <si>
+    <t>Number of days for 100% of nutrients to mix</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1671,6 +1671,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1716,7 +1725,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1777,14 +1786,29 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -3307,7 +3331,7 @@
         <v>57</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>93</v>
@@ -4021,8 +4045,8 @@
   <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4037,22 +4061,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -4060,64 +4084,64 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="29" t="s">
         <v>93</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="C3" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="D3" s="14" t="s">
+      <c r="C3" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="D3" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="E3" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" s="29" t="s">
         <v>93</v>
       </c>
       <c r="H3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>250</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="C4" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="20" t="s">
         <v>93</v>
       </c>
       <c r="G4" s="7"/>
@@ -4126,22 +4150,22 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>241</v>
-      </c>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" s="10" t="s">
+      <c r="D5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="20" t="s">
         <v>93</v>
       </c>
       <c r="G5" s="7"/>
@@ -4151,22 +4175,22 @@
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>231</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>251</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="C6" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="20" t="s">
         <v>93</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -4175,22 +4199,22 @@
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>230</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>252</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="C7" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="20" t="s">
         <v>93</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -4199,22 +4223,22 @@
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>242</v>
-      </c>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="21" t="s">
         <v>233</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="20" t="s">
         <v>93</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -4223,22 +4247,22 @@
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="B9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>265</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="13">
+      <c r="C9" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="21">
         <v>150</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="20" t="s">
         <v>93</v>
       </c>
       <c r="G9" s="7"/>
@@ -4247,22 +4271,22 @@
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>243</v>
-      </c>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="21" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="13">
+      <c r="D10" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="20" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="7"/>
@@ -4271,22 +4295,22 @@
       </c>
     </row>
     <row r="11" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B11" s="14" t="s">
+      <c r="A11" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B11" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="D11" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="28">
         <v>0.5</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G11"/>
@@ -4296,22 +4320,22 @@
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B12" s="14" t="s">
+      <c r="A12" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="28">
         <v>0.5</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G12"/>
@@ -4321,22 +4345,22 @@
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B13" s="14" t="s">
+      <c r="A13" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="28">
         <v>0.2</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="F13" s="29" t="s">
         <v>117</v>
       </c>
       <c r="H13" s="3" t="s">
@@ -4344,22 +4368,22 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B14" s="14" t="s">
+      <c r="A14" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="21" t="s">
         <v>234</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="28">
         <v>0</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="29" t="s">
         <v>117</v>
       </c>
       <c r="H14" s="3" t="s">
@@ -4367,22 +4391,22 @@
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B15" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>261</v>
-      </c>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="D15" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="28">
         <v>0.01</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="29" t="s">
         <v>117</v>
       </c>
       <c r="H15" s="3" t="s">
@@ -4390,22 +4414,22 @@
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B16" s="14" t="s">
+      <c r="A16" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>199</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="28">
         <v>0.01</v>
       </c>
-      <c r="F16" s="9" t="s">
+      <c r="F16" s="29" t="s">
         <v>117</v>
       </c>
       <c r="H16" s="3" t="s">
@@ -4414,22 +4438,22 @@
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B17" s="14" t="s">
+      <c r="A17" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17" s="28" t="s">
         <v>205</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="28">
         <v>0.05</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="F17" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G17"/>
@@ -4439,22 +4463,22 @@
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B18" s="14" t="s">
+      <c r="A18" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B18" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="28">
         <v>0.05</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G18"/>
@@ -4463,22 +4487,22 @@
       </c>
     </row>
     <row r="19" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14" t="s">
-        <v>244</v>
-      </c>
-      <c r="B19" s="14" t="s">
+      <c r="A19" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="B19" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E19" s="14">
+      <c r="C19" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="28">
         <v>0</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G19"/>
@@ -4488,22 +4512,22 @@
       <c r="I19"/>
     </row>
     <row r="20" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B20" s="14" t="s">
+      <c r="A20" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B20" s="28" t="s">
         <v>202</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>260</v>
-      </c>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D20" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="28">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G20"/>
@@ -4513,22 +4537,22 @@
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>247</v>
-      </c>
-      <c r="B21" s="14" t="s">
+      <c r="A21" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B21" s="28" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="28">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G21"/>
@@ -4538,22 +4562,22 @@
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="B22" s="14" t="s">
+      <c r="A22" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B22" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="14">
+      <c r="C22" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E22" s="28">
         <v>10</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G22"/>
@@ -4563,22 +4587,22 @@
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="C23" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="D23" s="13" t="s">
+      <c r="C23" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="D23" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="28">
         <v>1</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G23"/>
@@ -4587,22 +4611,22 @@
       </c>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B24" s="14" t="s">
+      <c r="A24" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B24" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="C24" s="13" t="s">
-        <v>259</v>
-      </c>
-      <c r="D24" s="13" t="s">
+      <c r="C24" s="21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D24" s="21" t="s">
         <v>235</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="28">
         <v>1</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G24"/>
@@ -4611,22 +4635,22 @@
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B25" s="14" t="s">
+      <c r="A25" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B25" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="C25" s="13" t="s">
-        <v>256</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="C25" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="D25" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="28">
         <v>0</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G25"/>
@@ -4636,22 +4660,22 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B26" s="14" t="s">
+      <c r="A26" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B26" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>257</v>
-      </c>
-      <c r="D26" s="14" t="s">
+      <c r="C26" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="D26" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="28">
         <v>0</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G26"/>
@@ -4661,22 +4685,22 @@
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B27" s="14" t="s">
+      <c r="A27" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B27" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C27" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="D27" s="14" t="s">
+      <c r="C27" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="D27" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="28">
         <v>100</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G27"/>
@@ -4686,22 +4710,22 @@
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B28" s="14" t="s">
+      <c r="A28" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="B28" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="C28" s="13" t="s">
-        <v>264</v>
-      </c>
-      <c r="D28" s="14" t="s">
+      <c r="C28" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="D28" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="28">
         <v>100</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G28"/>
@@ -4710,22 +4734,22 @@
       </c>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B29" s="14" t="s">
+      <c r="A29" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="C29" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="D29" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="26" t="s">
+      <c r="D29" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G29"/>
@@ -4735,22 +4759,22 @@
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B30" s="14" t="s">
+      <c r="A30" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B30" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="D30" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E30" s="26" t="s">
+      <c r="D30" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G30"/>
@@ -4760,22 +4784,22 @@
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B31" s="14" t="s">
+      <c r="A31" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B31" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31" s="26" t="s">
+      <c r="D31" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G31"/>
@@ -4785,22 +4809,22 @@
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B32" s="14" t="s">
+      <c r="A32" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B32" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C32" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E32" s="26" t="s">
+      <c r="D32" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G32"/>
@@ -4810,22 +4834,22 @@
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B33" s="14" t="s">
+      <c r="A33" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B33" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E33" s="26" t="s">
+      <c r="D33" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G33"/>
@@ -4835,22 +4859,22 @@
       <c r="I33"/>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B34" s="14" t="s">
+      <c r="A34" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B34" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E34" s="26" t="s">
+      <c r="D34" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E34" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G34"/>
@@ -4860,22 +4884,22 @@
       <c r="I34"/>
     </row>
     <row r="35" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
-        <v>246</v>
-      </c>
-      <c r="B35" s="14" t="s">
+      <c r="A35" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="B35" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="C35" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="D35" s="14" t="s">
+      <c r="C35" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="D35" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="28">
         <v>600</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G35"/>
@@ -4885,22 +4909,22 @@
       <c r="I35"/>
     </row>
     <row r="36" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B36" s="14" t="s">
+      <c r="A36" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B36" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C36" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E36" s="14">
+      <c r="C36" s="28" t="s">
+        <v>253</v>
+      </c>
+      <c r="D36" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="28">
         <v>0.1</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G36"/>
@@ -4910,22 +4934,22 @@
       <c r="I36"/>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="B37" s="14" t="s">
+      <c r="A37" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B37" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="C37" s="14" t="s">
+      <c r="C37" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E37" s="14">
+      <c r="D37" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="28">
         <v>0.1</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G37"/>
@@ -4989,7 +5013,7 @@
       <c r="I42" s="22"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="28" t="s">
+      <c r="A43" s="27" t="s">
         <v>181</v>
       </c>
       <c r="B43" s="24"/>
@@ -4999,7 +5023,7 @@
       <c r="D43" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="27" t="s">
+      <c r="E43" s="26" t="s">
         <v>163</v>
       </c>
       <c r="F43" s="18" t="s">

</xml_diff>

<commit_message>
more changes to Parameter Table and figures for paper
</commit_message>
<xml_diff>
--- a/Parameter Table.xlsx
+++ b/Parameter Table.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="272">
   <si>
     <t>Parameter</t>
   </si>
@@ -1041,7 +1041,7 @@
   </si>
   <si>
     <r>
-      <t>mg L</t>
+      <t>mg N L</t>
     </r>
     <r>
       <rPr>
@@ -1055,8 +1055,30 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>mg N L</t>
+    <t>g DW</t>
+  </si>
+  <si>
+    <r>
+      <t>(g DW m</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
     </r>
     <r>
       <rPr>
@@ -1070,30 +1092,104 @@
     </r>
   </si>
   <si>
-    <t>g DW</t>
-  </si>
-  <si>
-    <r>
-      <t>(g DW m</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>)</t>
+    <t>????</t>
+  </si>
+  <si>
+    <t>Shape parameter 1 for beta distribution of wind strength</t>
+  </si>
+  <si>
+    <t>Shape parameter 2 of beta distribution of wind strength</t>
+  </si>
+  <si>
+    <t>Water body characteristic</t>
+  </si>
+  <si>
+    <t>Initialization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seasonality </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth </t>
+  </si>
+  <si>
+    <t>Movement, vegetative</t>
+  </si>
+  <si>
+    <t>Movement, wind</t>
+  </si>
+  <si>
+    <t>Nutrient uptake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overwintering </t>
+  </si>
+  <si>
+    <t>Nutrient mixing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Water body surface area </t>
+  </si>
+  <si>
+    <t>Percent of water body surface covered by FP, initial</t>
+  </si>
+  <si>
+    <t>Percent of water body surface covered by SAV, initial</t>
+  </si>
+  <si>
+    <t>Maximum relative growth rate of FP</t>
+  </si>
+  <si>
+    <t>Proportion of FP biomass surviving overwintering</t>
+  </si>
+  <si>
+    <t>Biomass, above which, wind will not move FP into cell</t>
+  </si>
+  <si>
+    <t>Biomass, above which, FP will not colonize focal cell</t>
+  </si>
+  <si>
+    <t>Biomass, above which, SAV will not colonize focal cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass of FP to colonize focal cell </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biomass of SAV to colonize focal cell </t>
+  </si>
+  <si>
+    <t>Nitrogen uptake rate by FP</t>
+  </si>
+  <si>
+    <t>Self (light) limitation of FP</t>
+  </si>
+  <si>
+    <t>Light attenuation in the water column</t>
+  </si>
+  <si>
+    <t>Neighbor biomass, above which, FP colonizes focal cell</t>
+  </si>
+  <si>
+    <t>Neighbor biomass, above which, SAV colonizes focal cell</t>
+  </si>
+  <si>
+    <t>Number of days in a growing season</t>
+  </si>
+  <si>
+    <t>Submerged plant biomass</t>
+  </si>
+  <si>
+    <t>Number of days for 100% of nutrients to mix</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Total nitrogen, current</t>
+  </si>
+  <si>
+    <r>
+      <t>mg N g DW</t>
     </r>
     <r>
       <rPr>
@@ -1105,96 +1201,34 @@
       </rPr>
       <t>-1</t>
     </r>
-  </si>
-  <si>
-    <t>????</t>
-  </si>
-  <si>
-    <t>Shape parameter 1 for beta distribution of wind strength</t>
-  </si>
-  <si>
-    <t>Shape parameter 2 of beta distribution of wind strength</t>
-  </si>
-  <si>
-    <t>Water body characteristic</t>
-  </si>
-  <si>
-    <t>Initialization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seasonality </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Growth </t>
-  </si>
-  <si>
-    <t>Movement, vegetative</t>
-  </si>
-  <si>
-    <t>Movement, wind</t>
-  </si>
-  <si>
-    <t>Nutrient uptake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overwintering </t>
-  </si>
-  <si>
-    <t>Nutrient mixing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Water body surface area </t>
-  </si>
-  <si>
-    <t>Percent of water body surface covered by FP, initial</t>
-  </si>
-  <si>
-    <t>Percent of water body surface covered by SAV, initial</t>
-  </si>
-  <si>
-    <t>Maximum relative growth rate of FP</t>
-  </si>
-  <si>
-    <t>Proportion of FP biomass surviving overwintering</t>
-  </si>
-  <si>
-    <t>Biomass, above which, wind will not move FP into cell</t>
-  </si>
-  <si>
-    <t>Biomass, above which, FP will not colonize focal cell</t>
-  </si>
-  <si>
-    <t>Biomass, above which, SAV will not colonize focal cell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass of FP to colonize focal cell </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biomass of SAV to colonize focal cell </t>
-  </si>
-  <si>
-    <t>Nitrogen uptake rate by FP</t>
-  </si>
-  <si>
-    <t>Self (light) limitation of FP</t>
-  </si>
-  <si>
-    <t>Light attenuation in the water column</t>
-  </si>
-  <si>
-    <t>Neighbor biomass, above which, FP colonizes focal cell</t>
-  </si>
-  <si>
-    <t>Neighbor biomass, above which, SAV colonizes focal cell</t>
-  </si>
-  <si>
-    <t>Number of days in a growing season</t>
-  </si>
-  <si>
-    <t>Submerged plant biomass</t>
-  </si>
-  <si>
-    <t>Number of days for 100% of nutrients to mix</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> d</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+  </si>
+  <si>
+    <t>Janse &amp; van Puijenbroek 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE PUT INTO A FOOTNOTE FOR THE TABLE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHANGE THE SOURCES TO NUMBERS THAT CAN </t>
   </si>
 </sst>
 </file>
@@ -1347,7 +1381,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1525,6 +1559,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1725,7 +1765,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1809,6 +1849,20 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2155,8 +2209,8 @@
   <dimension ref="A1:G86"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C32" sqref="C32"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57:G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3331,7 +3385,7 @@
         <v>57</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D54" s="9" t="s">
         <v>93</v>
@@ -3393,48 +3447,48 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
+      <c r="A57" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C57" s="14" t="s">
+      <c r="C57" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="D57" s="9" t="s">
+      <c r="D57" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="E57" s="9">
+      <c r="E57" s="38">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F57" s="9" t="s">
+      <c r="F57" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G57" s="38" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
+      <c r="A58" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="D58" s="9" t="s">
+      <c r="D58" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="E58" s="9">
+      <c r="E58" s="38">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F58" s="9" t="s">
+      <c r="F58" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="G58" s="38" t="s">
         <v>173</v>
       </c>
     </row>
@@ -4042,11 +4096,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4054,13 +4108,13 @@
     <col min="1" max="1" width="22.42578125" style="15" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="15" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.140625" style="15" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" style="11" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>140</v>
       </c>
@@ -4083,7 +4137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="28" t="s">
         <v>212</v>
       </c>
@@ -4104,7 +4158,7 @@
       </c>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="28" t="s">
         <v>212</v>
       </c>
@@ -4112,7 +4166,7 @@
         <v>209</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D3" s="28" t="s">
         <v>232</v>
@@ -4125,42 +4179,39 @@
       </c>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="B4" s="21" t="s">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="B4" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>267</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="D4" s="21" t="s">
+      <c r="C5" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>159</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F4" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>93</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>93</v>
@@ -4170,164 +4221,163 @@
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="B6" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="7"/>
-    </row>
-    <row r="6" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="21" t="s">
+      <c r="C6" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
         <v>241</v>
       </c>
-      <c r="B6" s="21" t="s">
-        <v>231</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>250</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6"/>
-    </row>
-    <row r="7" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>230</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>251</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7"/>
-    </row>
-    <row r="8" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="H8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="B9" s="21" t="s">
+      <c r="B10" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="21">
+      <c r="C10" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="21">
         <v>150</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="E10" s="21">
-        <v>5</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>93</v>
       </c>
       <c r="G10" s="7"/>
       <c r="H10" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="B11" s="21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="C11" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="21">
+        <v>5</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="B12" s="28" t="s">
         <v>198</v>
       </c>
-      <c r="C11" s="28" t="s">
-        <v>252</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="E11" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11"/>
-      <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11"/>
-    </row>
-    <row r="12" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="B12" s="28" t="s">
-        <v>197</v>
-      </c>
       <c r="C12" s="28" t="s">
-        <v>111</v>
+        <v>251</v>
       </c>
       <c r="D12" s="28" t="s">
         <v>116</v>
@@ -4340,91 +4390,99 @@
       </c>
       <c r="G12"/>
       <c r="H12" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I12"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>234</v>
+        <v>111</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>116</v>
       </c>
       <c r="E13" s="28">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="29" t="s">
         <v>117</v>
       </c>
+      <c r="G13"/>
       <c r="H13" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="I13"/>
+      <c r="J13" s="7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B14" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E14" s="28">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F14" s="29" t="s">
         <v>117</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B15" s="28" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>236</v>
+        <v>121</v>
+      </c>
+      <c r="D15" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="E15" s="28">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="F15" s="29" t="s">
         <v>117</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B16" s="28" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E16" s="28">
         <v>0.01</v>
@@ -4433,44 +4491,42 @@
         <v>117</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="7"/>
-    </row>
-    <row r="17" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="D17" s="28" t="s">
-        <v>116</v>
+        <v>235</v>
       </c>
       <c r="E17" s="28">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F17" s="29" t="s">
         <v>117</v>
       </c>
-      <c r="G17"/>
-      <c r="H17" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17"/>
+      <c r="H17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B18" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>116</v>
@@ -4483,145 +4539,146 @@
       </c>
       <c r="G18"/>
       <c r="H18" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+      <c r="I18"/>
+    </row>
+    <row r="19" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="28" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B19" s="28" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>261</v>
+        <v>127</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>93</v>
+        <v>116</v>
       </c>
       <c r="E19" s="28">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="F19" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G19"/>
-      <c r="H19" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19"/>
-    </row>
-    <row r="20" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H19" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B20" s="28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D20" s="28" t="s">
-        <v>236</v>
+        <v>93</v>
       </c>
       <c r="E20" s="28">
-        <v>5.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F20" s="29" t="s">
         <v>117</v>
       </c>
       <c r="G20"/>
       <c r="H20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E21" s="34">
+        <v>70</v>
+      </c>
+      <c r="F21" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="G21" s="36"/>
+      <c r="H21" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="I20"/>
-    </row>
-    <row r="21" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="28" t="s">
-        <v>246</v>
-      </c>
-      <c r="B21" s="28" t="s">
+      <c r="I21"/>
+    </row>
+    <row r="22" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="B22" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C22" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="D21" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="E21" s="28">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21"/>
-      <c r="H21" s="3" t="s">
+      <c r="D22" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E22" s="34">
+        <v>70</v>
+      </c>
+      <c r="F22" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="G22" s="36"/>
+      <c r="H22" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="I21"/>
-    </row>
-    <row r="22" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="B22" s="28" t="s">
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="B23" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>266</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="28">
+      <c r="C23" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="D23" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="28">
         <v>10</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="G22"/>
-      <c r="H22" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="I22"/>
-    </row>
-    <row r="23" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="28" t="s">
-        <v>244</v>
-      </c>
-      <c r="B23" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="C23" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="D23" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="E23" s="28">
-        <v>1</v>
       </c>
       <c r="F23" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G23"/>
-      <c r="H23" s="6" t="s">
-        <v>40</v>
-      </c>
+      <c r="H23" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23"/>
     </row>
     <row r="24" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B24" s="28" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="C24" s="21" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E24" s="28">
         <v>1</v>
@@ -4631,43 +4688,42 @@
       </c>
       <c r="G24"/>
       <c r="H24" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B25" s="28" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C25" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>232</v>
+        <v>257</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>234</v>
       </c>
       <c r="E25" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F25" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G25"/>
       <c r="H25" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I25"/>
+        <v>37</v>
+      </c>
     </row>
     <row r="26" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C26" s="21" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D26" s="28" t="s">
         <v>232</v>
@@ -4680,44 +4736,44 @@
       </c>
       <c r="G26"/>
       <c r="H26" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I26"/>
     </row>
     <row r="27" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B27" s="28" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C27" s="21" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="D27" s="28" t="s">
         <v>232</v>
       </c>
       <c r="E27" s="28">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G27"/>
       <c r="H27" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D28" s="28" t="s">
         <v>232</v>
@@ -4730,218 +4786,218 @@
       </c>
       <c r="G28"/>
       <c r="H28" s="6" t="s">
-        <v>35</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="I28"/>
     </row>
     <row r="29" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B29" s="28" t="s">
-        <v>222</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>238</v>
+        <v>214</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>262</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="E29" s="28">
+        <v>100</v>
       </c>
       <c r="F29" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G29"/>
       <c r="H29" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I29"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="30" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B30" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D30" s="28" t="s">
         <v>93</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F30" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G30"/>
       <c r="H30" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B31" s="28" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C31" s="28" t="s">
-        <v>145</v>
+        <v>238</v>
       </c>
       <c r="D31" s="28" t="s">
         <v>93</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F31" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G31"/>
       <c r="H31" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B32" s="28" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D32" s="28" t="s">
         <v>93</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F32" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G32"/>
-      <c r="H32" s="3" t="s">
-        <v>81</v>
+      <c r="H32" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B33" s="28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D33" s="28" t="s">
         <v>93</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F33" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G33"/>
       <c r="H33" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I33"/>
     </row>
     <row r="34" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B34" s="28" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D34" s="28" t="s">
         <v>93</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F34" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G34"/>
-      <c r="H34" s="6" t="s">
-        <v>80</v>
+      <c r="H34" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="I34"/>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="28" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B35" s="28" t="s">
-        <v>228</v>
-      </c>
-      <c r="C35" s="21" t="s">
-        <v>254</v>
+        <v>224</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>146</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>232</v>
-      </c>
-      <c r="E35" s="28">
-        <v>600</v>
+        <v>93</v>
+      </c>
+      <c r="E35" s="31" t="s">
+        <v>236</v>
       </c>
       <c r="F35" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G35"/>
-      <c r="H35" s="3" t="s">
-        <v>84</v>
+      <c r="H35" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="I35"/>
     </row>
-    <row r="36" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="28" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B36" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="C36" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="C36" s="21" t="s">
         <v>253</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>93</v>
+        <v>232</v>
       </c>
       <c r="E36" s="28">
-        <v>0.1</v>
+        <v>600</v>
       </c>
       <c r="F36" s="30" t="s">
         <v>139</v>
       </c>
       <c r="G36"/>
       <c r="H36" s="3" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="I36"/>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="28" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B37" s="28" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>134</v>
+        <v>252</v>
       </c>
       <c r="D37" s="28" t="s">
         <v>93</v>
@@ -4954,19 +5010,33 @@
       </c>
       <c r="G37"/>
       <c r="H37" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I37"/>
+    </row>
+    <row r="38" spans="1:9" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="B38" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D38" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" s="28">
+        <v>0.1</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38"/>
+      <c r="H38" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
-      <c r="D38" s="21"/>
-      <c r="E38" s="21"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
     </row>
     <row r="39" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="21"/>
@@ -5012,46 +5082,36 @@
       <c r="H42" s="22"/>
       <c r="I42" s="22"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="27" t="s">
+    <row r="43" spans="1:9" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="17" t="s">
+      <c r="B44" s="24"/>
+      <c r="C44" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="D43" s="24" t="s">
+      <c r="D44" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E44" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="F43" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="H43" s="19" t="s">
+      <c r="F44" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="H44" s="19" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
-        <v>181</v>
-      </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>163</v>
-      </c>
-      <c r="F44" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="H44" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
@@ -5060,7 +5120,7 @@
       </c>
       <c r="B45" s="14"/>
       <c r="C45" s="16" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D45" s="14" t="s">
         <v>151</v>
@@ -5072,7 +5132,7 @@
         <v>93</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -5081,7 +5141,7 @@
       </c>
       <c r="B46" s="14"/>
       <c r="C46" s="16" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>151</v>
@@ -5093,31 +5153,29 @@
         <v>93</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="B47" s="13"/>
+      <c r="B47" s="14"/>
       <c r="C47" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="D47" s="25" t="s">
-        <v>100</v>
+        <v>188</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>151</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="F47" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G47" s="7"/>
-      <c r="H47" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I47" s="7"/>
+      <c r="H47" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
@@ -5125,7 +5183,7 @@
       </c>
       <c r="B48" s="13"/>
       <c r="C48" s="16" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D48" s="25" t="s">
         <v>100</v>
@@ -5138,30 +5196,30 @@
       </c>
       <c r="G48" s="7"/>
       <c r="H48" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I48" s="7"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B49" s="13"/>
-      <c r="C49" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D49" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="13">
-        <v>1</v>
+      <c r="C49" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>100</v>
       </c>
       <c r="F49" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G49" s="7"/>
       <c r="H49" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I49" s="7"/>
     </row>
@@ -5171,20 +5229,20 @@
       </c>
       <c r="B50" s="13"/>
       <c r="C50" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>100</v>
+        <v>89</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E50" s="13">
+        <v>1</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G50" s="7"/>
       <c r="H50" s="6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I50" s="7"/>
     </row>
@@ -5193,8 +5251,8 @@
         <v>164</v>
       </c>
       <c r="B51" s="13"/>
-      <c r="C51" s="16" t="s">
-        <v>190</v>
+      <c r="C51" s="13" t="s">
+        <v>189</v>
       </c>
       <c r="D51" s="25" t="s">
         <v>100</v>
@@ -5207,7 +5265,7 @@
       </c>
       <c r="G51" s="7"/>
       <c r="H51" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I51" s="7"/>
     </row>
@@ -5216,21 +5274,21 @@
         <v>164</v>
       </c>
       <c r="B52" s="13"/>
-      <c r="C52" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>93</v>
+      <c r="C52" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>100</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>163</v>
+        <v>100</v>
       </c>
       <c r="F52" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G52" s="7"/>
       <c r="H52" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I52" s="7"/>
     </row>
@@ -5240,20 +5298,20 @@
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E53" s="13">
-        <v>100</v>
+        <v>95</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E53" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="F53" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G53" s="7"/>
       <c r="H53" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I53" s="7"/>
     </row>
@@ -5263,20 +5321,20 @@
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>163</v>
+        <v>96</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E54" s="13">
+        <v>100</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G54" s="7"/>
       <c r="H54" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I54" s="7"/>
     </row>
@@ -5286,20 +5344,20 @@
       </c>
       <c r="B55" s="13"/>
       <c r="C55" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="E55" s="13">
-        <v>100</v>
+        <v>98</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E55" s="25" t="s">
+        <v>163</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G55" s="7"/>
       <c r="H55" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I55" s="7"/>
     </row>
@@ -5309,20 +5367,20 @@
       </c>
       <c r="B56" s="13"/>
       <c r="C56" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D56" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="E56" s="25" t="s">
-        <v>163</v>
+        <v>99</v>
+      </c>
+      <c r="D56" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E56" s="13">
+        <v>100</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>93</v>
       </c>
       <c r="G56" s="7"/>
       <c r="H56" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I56" s="7"/>
     </row>
@@ -5332,7 +5390,7 @@
       </c>
       <c r="B57" s="13"/>
       <c r="C57" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D57" s="13" t="s">
         <v>93</v>
@@ -5345,7 +5403,7 @@
       </c>
       <c r="G57" s="7"/>
       <c r="H57" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I57" s="7"/>
     </row>
@@ -5355,7 +5413,7 @@
       </c>
       <c r="B58" s="13"/>
       <c r="C58" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D58" s="13" t="s">
         <v>93</v>
@@ -5368,7 +5426,7 @@
       </c>
       <c r="G58" s="7"/>
       <c r="H58" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I58" s="7"/>
     </row>
@@ -5378,7 +5436,7 @@
       </c>
       <c r="B59" s="13"/>
       <c r="C59" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>93</v>
@@ -5391,7 +5449,7 @@
       </c>
       <c r="G59" s="7"/>
       <c r="H59" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I59" s="7"/>
     </row>
@@ -5401,7 +5459,7 @@
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D60" s="13" t="s">
         <v>93</v>
@@ -5414,7 +5472,7 @@
       </c>
       <c r="G60" s="7"/>
       <c r="H60" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I60" s="7"/>
     </row>
@@ -5424,10 +5482,10 @@
       </c>
       <c r="B61" s="13"/>
       <c r="C61" s="13" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>152</v>
+        <v>93</v>
       </c>
       <c r="E61" s="25" t="s">
         <v>163</v>
@@ -5437,7 +5495,7 @@
       </c>
       <c r="G61" s="7"/>
       <c r="H61" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I61" s="7"/>
     </row>
@@ -5447,7 +5505,7 @@
       </c>
       <c r="B62" s="13"/>
       <c r="C62" s="13" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D62" s="13" t="s">
         <v>152</v>
@@ -5460,7 +5518,7 @@
       </c>
       <c r="G62" s="7"/>
       <c r="H62" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I62" s="7"/>
     </row>
@@ -5470,7 +5528,7 @@
       </c>
       <c r="B63" s="13"/>
       <c r="C63" s="13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D63" s="13" t="s">
         <v>152</v>
@@ -5483,7 +5541,7 @@
       </c>
       <c r="G63" s="7"/>
       <c r="H63" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I63" s="7"/>
     </row>
@@ -5493,7 +5551,7 @@
       </c>
       <c r="B64" s="13"/>
       <c r="C64" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D64" s="13" t="s">
         <v>152</v>
@@ -5506,7 +5564,7 @@
       </c>
       <c r="G64" s="7"/>
       <c r="H64" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I64" s="7"/>
     </row>
@@ -5516,7 +5574,7 @@
       </c>
       <c r="B65" s="13"/>
       <c r="C65" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D65" s="13" t="s">
         <v>152</v>
@@ -5529,30 +5587,32 @@
       </c>
       <c r="G65" s="7"/>
       <c r="H65" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I65" s="7"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="D66" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I65" s="7"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="B66" s="14"/>
-      <c r="C66" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E66" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="F66" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>43</v>
-      </c>
+      <c r="I66" s="7"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="14" t="s">
@@ -5560,7 +5620,7 @@
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>116</v>
@@ -5572,7 +5632,7 @@
         <v>117</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -5581,7 +5641,7 @@
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D68" s="14" t="s">
         <v>116</v>
@@ -5593,7 +5653,7 @@
         <v>117</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -5602,19 +5662,19 @@
       </c>
       <c r="B69" s="14"/>
       <c r="C69" s="14" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D69" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E69" s="14">
-        <v>0.01</v>
+        <v>0.5</v>
       </c>
       <c r="F69" s="9" t="s">
         <v>117</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -5635,7 +5695,7 @@
         <v>117</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -5656,7 +5716,7 @@
         <v>117</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -5665,19 +5725,19 @@
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="14" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D72" s="14" t="s">
-        <v>154</v>
+        <v>120</v>
       </c>
       <c r="E72" s="14">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="F72" s="9" t="s">
         <v>117</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -5686,7 +5746,7 @@
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D73" s="14" t="s">
         <v>154</v>
@@ -5698,7 +5758,7 @@
         <v>117</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -5707,7 +5767,7 @@
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D74" s="14" t="s">
         <v>154</v>
@@ -5719,7 +5779,7 @@
         <v>117</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -5728,40 +5788,40 @@
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
       <c r="E75" s="14">
-        <v>0.02</v>
+        <v>0.2</v>
       </c>
       <c r="F75" s="9" t="s">
         <v>117</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B76" s="14"/>
       <c r="C76" s="14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D76" s="14" t="s">
         <v>120</v>
       </c>
       <c r="E76" s="14">
-        <v>5.0000000000000001E-3</v>
+        <v>0.02</v>
       </c>
       <c r="F76" s="9" t="s">
         <v>117</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -5770,7 +5830,7 @@
       </c>
       <c r="B77" s="14"/>
       <c r="C77" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D77" s="14" t="s">
         <v>120</v>
@@ -5782,7 +5842,7 @@
         <v>117</v>
       </c>
       <c r="H77" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -5791,7 +5851,7 @@
       </c>
       <c r="B78" s="14"/>
       <c r="C78" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D78" s="14" t="s">
         <v>120</v>
@@ -5803,7 +5863,7 @@
         <v>117</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -5812,19 +5872,19 @@
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14" t="s">
-        <v>191</v>
+        <v>133</v>
       </c>
       <c r="D79" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="E79" s="14" t="s">
-        <v>93</v>
+      <c r="E79" s="14">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>93</v>
+        <v>117</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -5833,7 +5893,7 @@
       </c>
       <c r="B80" s="14"/>
       <c r="C80" s="14" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D80" s="14" t="s">
         <v>120</v>
@@ -5845,7 +5905,7 @@
         <v>93</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -5854,7 +5914,7 @@
       </c>
       <c r="B81" s="14"/>
       <c r="C81" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D81" s="14" t="s">
         <v>120</v>
@@ -5866,7 +5926,7 @@
         <v>93</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -5875,7 +5935,7 @@
       </c>
       <c r="B82" s="14"/>
       <c r="C82" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D82" s="14" t="s">
         <v>120</v>
@@ -5887,7 +5947,7 @@
         <v>93</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -5896,7 +5956,7 @@
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="14" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D83" s="14" t="s">
         <v>120</v>
@@ -5908,28 +5968,28 @@
         <v>93</v>
       </c>
       <c r="H83" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="14" t="s">
-        <v>136</v>
+        <v>195</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E84" s="14">
-        <v>0.1</v>
-      </c>
-      <c r="F84" s="2" t="s">
-        <v>139</v>
+        <v>120</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="F84" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -5938,7 +5998,7 @@
       </c>
       <c r="B85" s="14"/>
       <c r="C85" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D85" s="14" t="s">
         <v>93</v>
@@ -5950,7 +6010,7 @@
         <v>139</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -5959,7 +6019,7 @@
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D86" s="14" t="s">
         <v>93</v>
@@ -5971,28 +6031,28 @@
         <v>139</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" s="14" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="14" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D87" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E87" s="25" t="s">
-        <v>163</v>
+      <c r="E87" s="14">
+        <v>0.1</v>
       </c>
       <c r="F87" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H87" s="6" t="s">
-        <v>77</v>
+      <c r="H87" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -6001,7 +6061,7 @@
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D88" s="14" t="s">
         <v>93</v>
@@ -6013,7 +6073,7 @@
         <v>139</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -6022,19 +6082,19 @@
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="14" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="D89" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E89" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="F89" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>83</v>
+      <c r="E89" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -6042,30 +6102,51 @@
         <v>175</v>
       </c>
       <c r="B90" s="14"/>
-      <c r="C90" s="13" t="s">
+      <c r="C90" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="D90" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E90" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="F90" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D90" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="E90" s="14" t="s">
+      <c r="D91" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="E91" s="14" t="s">
         <v>178</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="H90" s="3" t="s">
+      <c r="H91" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="14"/>
-      <c r="B91" s="14"/>
-      <c r="C91" s="14"/>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
-      <c r="F91" s="9"/>
-      <c r="H91" s="3"/>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="14"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="9"/>
+      <c r="H92" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>